<commit_message>
Luanched the version 0.9
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unesco.sharepoint.com/sites/MontevideoTeam/Shared Documents/MaB/00.Database/1.MaB-API/MaB-API/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1131" documentId="8_{0D84168F-6C97-4B71-9D33-29523ED29034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82CCBEAD-FD33-47A8-80B9-F2A364AA84A7}"/>
+  <xr:revisionPtr revIDLastSave="1134" documentId="8_{0D84168F-6C97-4B71-9D33-29523ED29034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{087E6374-F065-4303-A1CF-1E8BD66E9B48}"/>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="-120" windowWidth="27915" windowHeight="16440" activeTab="1" xr2:uid="{85CD61FC-0185-45B9-BBE6-1C74E6F4F638}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{85CD61FC-0185-45B9-BBE6-1C74E6F4F638}"/>
   </bookViews>
   <sheets>
     <sheet name="available_lst" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2121" uniqueCount="849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2122" uniqueCount="850">
   <si>
     <t>id</t>
   </si>
@@ -2585,6 +2585,9 @@
   </si>
   <si>
     <t>/IberoAmericaMAB/surface/WITHDRAW/MEX-Islas_Del_Golfo_De_California.geojson</t>
+  </si>
+  <si>
+    <t>Withdraw in 2020</t>
   </si>
 </sst>
 </file>
@@ -2687,15 +2690,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="43">
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2808,6 +2802,15 @@
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2842,68 +2845,68 @@
     <tableColumn id="1" xr3:uid="{31D6180E-CD56-41CE-AA77-F64999A8E024}" name="id" dataDxfId="40"/>
     <tableColumn id="2" xr3:uid="{88B7A4E9-9D81-4869-B0BA-27D4F1E534D6}" name="country" dataDxfId="39"/>
     <tableColumn id="3" xr3:uid="{B63687E4-4798-4C9B-822B-797895EC75C1}" name="br_name" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{3921AE67-CDB0-45FC-B792-B73A520BE3B0}" name="geojson_surface" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{5E4A03E4-95CE-4932-ADEA-694E5B8ED7BE}" name="surface_file_location" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{97CC4F7A-D6C6-4D5A-9E04-BB6FA6550518}" name="geojson_core" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{76576057-7CF0-41D9-9125-7899A1DB1C95}" name="geojson_buffer" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{B6A0DD57-B933-43DC-BC0A-C340D94FF0FC}" name="comment" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{3921AE67-CDB0-45FC-B792-B73A520BE3B0}" name="geojson_surface" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{5E4A03E4-95CE-4932-ADEA-694E5B8ED7BE}" name="surface_file_location" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{97CC4F7A-D6C6-4D5A-9E04-BB6FA6550518}" name="geojson_core" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{76576057-7CF0-41D9-9125-7899A1DB1C95}" name="geojson_buffer" dataDxfId="34"/>
+    <tableColumn id="8" xr3:uid="{B6A0DD57-B933-43DC-BC0A-C340D94FF0FC}" name="comment" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0910542C-EA3A-4BF2-9103-F97D91704A02}" name="Table3" displayName="Table3" ref="A1:K137" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0910542C-EA3A-4BF2-9103-F97D91704A02}" name="Table3" displayName="Table3" ref="A1:K137" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A1:K137" xr:uid="{0910542C-EA3A-4BF2-9103-F97D91704A02}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K137">
     <sortCondition ref="A1:A137"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="10" xr3:uid="{5EFDF94E-758C-4ECF-9E1E-BFA9871CE014}" name="status" dataDxfId="33"/>
-    <tableColumn id="1" xr3:uid="{770D4E21-9A0B-47DD-8DF5-E4304D959315}" name="id" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{02E8B95F-8B50-4DB8-9FC1-4AD35772B144}" name="country" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{E97E4F7C-CA5F-4124-A9A9-8692216C7BB4}" name="iso2c" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{94F79DF6-66D0-42A0-8D28-F20A9FF47A6F}" name="iso3c" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{4C4EEF9C-D388-428D-A24C-0629A9447E3A}" name="name" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{68C0B232-8561-4059-A5E3-4A45760254F2}" name="designated_year" dataDxfId="27"/>
-    <tableColumn id="11" xr3:uid="{7FDCC376-33B1-456B-AC81-1C7A4952D958}" name="unesco_url" dataDxfId="26"/>
-    <tableColumn id="12" xr3:uid="{0333D1A1-7B00-463A-9B93-17B6A2B16FEF}" name="handle" dataDxfId="25"/>
-    <tableColumn id="13" xr3:uid="{6D0F62AB-EE01-42EE-989F-4400D6328D5D}" name="periodic_reviews_available" dataDxfId="24"/>
-    <tableColumn id="14" xr3:uid="{B28AEA32-51EC-48C5-9BA6-EF26AC6E7D8A}" name="lastupdate_date" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{5EFDF94E-758C-4ECF-9E1E-BFA9871CE014}" name="status" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{770D4E21-9A0B-47DD-8DF5-E4304D959315}" name="id" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{02E8B95F-8B50-4DB8-9FC1-4AD35772B144}" name="country" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{E97E4F7C-CA5F-4124-A9A9-8692216C7BB4}" name="iso2c" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{94F79DF6-66D0-42A0-8D28-F20A9FF47A6F}" name="iso3c" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{4C4EEF9C-D388-428D-A24C-0629A9447E3A}" name="name" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{68C0B232-8561-4059-A5E3-4A45760254F2}" name="designated_year" dataDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{7FDCC376-33B1-456B-AC81-1C7A4952D958}" name="unesco_url" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{0333D1A1-7B00-463A-9B93-17B6A2B16FEF}" name="handle" dataDxfId="22"/>
+    <tableColumn id="13" xr3:uid="{6D0F62AB-EE01-42EE-989F-4400D6328D5D}" name="periodic_reviews_available" dataDxfId="21"/>
+    <tableColumn id="14" xr3:uid="{B28AEA32-51EC-48C5-9BA6-EF26AC6E7D8A}" name="lastupdate_date" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0AE299EC-B7D0-48E0-B3DD-2D0A91C1B68D}" name="Table4" displayName="Table4" ref="A1:H11" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0AE299EC-B7D0-48E0-B3DD-2D0A91C1B68D}" name="Table4" displayName="Table4" ref="A1:H11" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:H11" xr:uid="{0AE299EC-B7D0-48E0-B3DD-2D0A91C1B68D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{9B819798-564C-412D-A4B0-1108C26DC434}" name="id" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{CA8C1EB9-A593-4DB1-A357-D84BFA7C788D}" name="country" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{4EE7F5F0-D781-49AF-B4EC-4A1A8E5E913D}" name="iso2c" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{4DD2419C-5216-4D5A-89E0-185C9B8C194B}" name="iso3c" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{207933B0-0BC5-4740-8D0A-3035C3F1C3C6}" name="name" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{B103807B-5A73-426D-9073-48F568716524}" name="year" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{8ECC6FAA-E805-4DE1-97BD-31C0C5EED76B}" name="transboundary" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{D02D9751-A22B-46DC-8BD5-66A6AAAE15C6}" name="comment" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{9B819798-564C-412D-A4B0-1108C26DC434}" name="id" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{CA8C1EB9-A593-4DB1-A357-D84BFA7C788D}" name="country" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{4EE7F5F0-D781-49AF-B4EC-4A1A8E5E913D}" name="iso2c" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{4DD2419C-5216-4D5A-89E0-185C9B8C194B}" name="iso3c" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{207933B0-0BC5-4740-8D0A-3035C3F1C3C6}" name="name" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{B103807B-5A73-426D-9073-48F568716524}" name="year" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{8ECC6FAA-E805-4DE1-97BD-31C0C5EED76B}" name="transboundary" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{D02D9751-A22B-46DC-8BD5-66A6AAAE15C6}" name="comment" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C3672DE5-898C-4457-BE21-7DB347AC1C86}" name="Table5" displayName="Table5" ref="A1:H23" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C3672DE5-898C-4457-BE21-7DB347AC1C86}" name="Table5" displayName="Table5" ref="A1:H23" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:H23" xr:uid="{C3672DE5-898C-4457-BE21-7DB347AC1C86}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{6D02B61A-B373-44F5-9078-F38DB1F4F060}" name="id" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{808668E7-3AAD-42AC-8DCE-7EBA1725DEF3}" name="name" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{1D013C41-AD67-44AF-95D9-85F43F6FDA94}" name="year" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{ACA2396B-471B-469E-9973-ACBB30A8F4B0}" name="sheet" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{916D6E94-F2C1-4887-AD7F-83009D1229BA}" name="key" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{EA2D7BCD-DFD9-4C2F-BBCD-08B0D8BBB01A}" name="old_value" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{61B28554-9F4D-42CF-83E2-9EF0145636B4}" name="new_value" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{6429DE8E-968A-4A34-8259-AEBA06A1520F}" name="comment" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{6D02B61A-B373-44F5-9078-F38DB1F4F060}" name="id" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{808668E7-3AAD-42AC-8DCE-7EBA1725DEF3}" name="name" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{1D013C41-AD67-44AF-95D9-85F43F6FDA94}" name="year" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{ACA2396B-471B-469E-9973-ACBB30A8F4B0}" name="sheet" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{916D6E94-F2C1-4887-AD7F-83009D1229BA}" name="key" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{EA2D7BCD-DFD9-4C2F-BBCD-08B0D8BBB01A}" name="old_value" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{61B28554-9F4D-42CF-83E2-9EF0145636B4}" name="new_value" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{6429DE8E-968A-4A34-8259-AEBA06A1520F}" name="comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3208,8 +3211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838904C7-54E8-4955-ACB3-A4B3D91077CE}">
   <dimension ref="A1:H137"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86:E86"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3360,59 +3363,63 @@
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>156</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>144</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6</v>
+        <v>147</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>718</v>
+        <v>828</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>705</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>5</v>
+        <v>281</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>7</v>
+        <v>440</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>719</v>
-      </c>
-      <c r="F9" s="3"/>
+        <v>848</v>
+      </c>
+      <c r="F9" s="2"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -3420,19 +3427,19 @@
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -3440,19 +3447,19 @@
     </row>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -3460,19 +3467,19 @@
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -3480,19 +3487,19 @@
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -3500,19 +3507,19 @@
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -3520,19 +3527,19 @@
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -3540,19 +3547,19 @@
     </row>
     <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -3560,19 +3567,19 @@
     </row>
     <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -3580,19 +3587,19 @@
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -3600,19 +3607,19 @@
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -3620,19 +3627,19 @@
     </row>
     <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -3640,19 +3647,19 @@
     </row>
     <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -3660,19 +3667,19 @@
     </row>
     <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -3680,19 +3687,19 @@
     </row>
     <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -3700,41 +3707,39 @@
     </row>
     <row r="25" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>156</v>
+        <v>88</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>144</v>
+        <v>87</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>147</v>
+        <v>81</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>828</v>
+        <v>733</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="3" t="s">
-        <v>518</v>
-      </c>
+      <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>157</v>
+        <v>90</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>144</v>
+        <v>87</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>149</v>
+        <v>83</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -3742,19 +3747,19 @@
     </row>
     <row r="27" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>144</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -3762,19 +3767,19 @@
     </row>
     <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>144</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -3782,19 +3787,19 @@
     </row>
     <row r="29" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>144</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -3802,19 +3807,19 @@
     </row>
     <row r="30" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>144</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -3822,19 +3827,19 @@
     </row>
     <row r="31" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -3842,19 +3847,19 @@
     </row>
     <row r="32" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>172</v>
+      <c r="C32" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>837</v>
+        <v>740</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -3862,19 +3867,19 @@
     </row>
     <row r="33" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>174</v>
+      <c r="C33" s="5" t="s">
+        <v>172</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>741</v>
+        <v>837</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
@@ -3882,19 +3887,19 @@
     </row>
     <row r="34" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>167</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
@@ -3902,19 +3907,19 @@
     </row>
     <row r="35" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>167</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
@@ -3922,19 +3927,19 @@
     </row>
     <row r="36" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>167</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -3942,19 +3947,19 @@
     </row>
     <row r="37" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>167</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -3962,19 +3967,19 @@
     </row>
     <row r="38" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>167</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -3982,19 +3987,19 @@
     </row>
     <row r="39" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>167</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -4002,19 +4007,19 @@
     </row>
     <row r="40" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>167</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
@@ -4022,19 +4027,19 @@
     </row>
     <row r="41" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>353</v>
+        <v>196</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>229</v>
+        <v>167</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>232</v>
+        <v>185</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
@@ -4042,19 +4047,19 @@
     </row>
     <row r="42" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>229</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -4062,19 +4067,19 @@
     </row>
     <row r="43" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>229</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
@@ -4082,19 +4087,19 @@
     </row>
     <row r="44" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>229</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -4102,19 +4107,19 @@
     </row>
     <row r="45" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>229</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -4122,19 +4127,19 @@
     </row>
     <row r="46" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>519</v>
+        <v>357</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -4142,19 +4147,19 @@
     </row>
     <row r="47" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>230</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -4162,19 +4167,19 @@
     </row>
     <row r="48" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>230</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -4182,19 +4187,19 @@
     </row>
     <row r="49" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>244</v>
+      <c r="C49" s="3" t="s">
+        <v>243</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>833</v>
+        <v>756</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -4202,19 +4207,19 @@
     </row>
     <row r="50" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>419</v>
+        <v>522</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>245</v>
+        <v>230</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>244</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>757</v>
+        <v>833</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
@@ -4222,19 +4227,19 @@
     </row>
     <row r="51" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>231</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -4242,19 +4247,19 @@
     </row>
     <row r="52" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>231</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
@@ -4262,19 +4267,19 @@
     </row>
     <row r="53" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>231</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
@@ -4282,19 +4287,19 @@
     </row>
     <row r="54" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>231</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -4302,19 +4307,19 @@
     </row>
     <row r="55" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>231</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
@@ -4322,19 +4327,19 @@
     </row>
     <row r="56" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>689</v>
+        <v>424</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>832</v>
+        <v>231</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>554</v>
+        <v>253</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>845</v>
+        <v>762</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
@@ -4342,10 +4347,10 @@
     </row>
     <row r="57" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>552</v>
+        <v>689</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>254</v>
+        <v>832</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>554</v>
@@ -4354,7 +4359,7 @@
         <v>516</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>763</v>
+        <v>845</v>
       </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
@@ -4362,19 +4367,19 @@
     </row>
     <row r="58" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>674</v>
+        <v>552</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>832</v>
+        <v>254</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>673</v>
+        <v>554</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>840</v>
+        <v>763</v>
       </c>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
@@ -4382,19 +4387,19 @@
     </row>
     <row r="59" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>524</v>
+        <v>674</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>257</v>
+        <v>832</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>258</v>
+        <v>673</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>764</v>
+        <v>840</v>
       </c>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
@@ -4402,19 +4407,19 @@
     </row>
     <row r="60" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>257</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -4422,19 +4427,19 @@
     </row>
     <row r="61" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>257</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
@@ -4442,19 +4447,19 @@
     </row>
     <row r="62" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>257</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>839</v>
+        <v>766</v>
       </c>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
@@ -4462,19 +4467,19 @@
     </row>
     <row r="63" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>264</v>
+      <c r="C63" s="3" t="s">
+        <v>263</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -4482,19 +4487,19 @@
     </row>
     <row r="64" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>544</v>
+      <c r="C64" s="5" t="s">
+        <v>264</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>829</v>
+        <v>838</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
@@ -4502,19 +4507,19 @@
     </row>
     <row r="65" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>257</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>265</v>
+        <v>544</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
@@ -4522,19 +4527,19 @@
     </row>
     <row r="66" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>697</v>
+        <v>532</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>832</v>
+        <v>257</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>696</v>
+        <v>265</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>844</v>
+        <v>830</v>
       </c>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -4542,19 +4547,19 @@
     </row>
     <row r="67" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>657</v>
+        <v>697</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>270</v>
+        <v>832</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>271</v>
+        <v>696</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>767</v>
+        <v>844</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -4562,19 +4567,19 @@
     </row>
     <row r="68" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>270</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
@@ -4582,19 +4587,19 @@
     </row>
     <row r="69" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>696</v>
+      <c r="C69" s="3" t="s">
+        <v>272</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>843</v>
+        <v>768</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
@@ -4602,19 +4607,19 @@
     </row>
     <row r="70" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>652</v>
+        <v>661</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>277</v>
+        <v>270</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>696</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>769</v>
+        <v>843</v>
       </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -4622,19 +4627,19 @@
     </row>
     <row r="71" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C71" s="5" t="s">
-        <v>696</v>
+      <c r="C71" s="3" t="s">
+        <v>277</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>842</v>
+        <v>769</v>
       </c>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
@@ -4642,19 +4647,19 @@
     </row>
     <row r="72" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>278</v>
+      <c r="C72" s="5" t="s">
+        <v>696</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>770</v>
+        <v>842</v>
       </c>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
@@ -4662,19 +4667,19 @@
     </row>
     <row r="73" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C73" s="5" t="s">
-        <v>279</v>
+      <c r="C73" s="3" t="s">
+        <v>278</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>834</v>
+        <v>770</v>
       </c>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
@@ -4682,19 +4687,19 @@
     </row>
     <row r="74" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>525</v>
+        <v>655</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>694</v>
+        <v>280</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>279</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>846</v>
+        <v>834</v>
       </c>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
@@ -4702,19 +4707,19 @@
     </row>
     <row r="75" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>534</v>
+        <v>525</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>383</v>
+        <v>276</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>295</v>
+        <v>694</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>771</v>
+        <v>846</v>
       </c>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
@@ -4722,59 +4727,59 @@
     </row>
     <row r="76" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>608</v>
+        <v>534</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>425</v>
+        <v>383</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="F76" s="2"/>
+        <v>771</v>
+      </c>
+      <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
     </row>
     <row r="77" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="C77" s="3" t="s">
-        <v>427</v>
+      <c r="C77" s="5" t="s">
+        <v>425</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>772</v>
-      </c>
-      <c r="F77" s="3"/>
+        <v>835</v>
+      </c>
+      <c r="F77" s="2"/>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
     </row>
     <row r="78" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>281</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
@@ -4782,19 +4787,19 @@
     </row>
     <row r="79" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>281</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
@@ -4802,19 +4807,19 @@
     </row>
     <row r="80" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>281</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
@@ -4822,19 +4827,19 @@
     </row>
     <row r="81" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>281</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
@@ -4842,19 +4847,19 @@
     </row>
     <row r="82" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>281</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
@@ -4862,19 +4867,19 @@
     </row>
     <row r="83" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>281</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
@@ -4882,19 +4887,19 @@
     </row>
     <row r="84" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>281</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
@@ -4902,19 +4907,19 @@
     </row>
     <row r="85" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>281</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>516</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
@@ -4922,21 +4927,21 @@
     </row>
     <row r="86" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>705</v>
+        <v>617</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>281</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>848</v>
-      </c>
-      <c r="F86" s="2"/>
+        <v>780</v>
+      </c>
+      <c r="F86" s="3"/>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
     </row>
@@ -5972,7 +5977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82114840-D598-4DC9-A4FB-2D6ADA307DFB}">
   <dimension ref="A1:K137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>